<commit_message>
* Refactored tests. * Implemented automatch.
</commit_message>
<xml_diff>
--- a/tests/test_artifacts/test_report_excel/benchmarks/test_report_excel.xlsx
+++ b/tests/test_artifacts/test_report_excel/benchmarks/test_report_excel.xlsx
@@ -9,10 +9,12 @@
   <sheets>
     <sheet name="schema_compare" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="values_compare" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="src_only" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="tgt_only" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="src_dup" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="tgt_dup" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="mismatches" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="matches" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="src_only" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="tgt_only" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="src_dup" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="tgt_dup" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -884,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -910,45 +912,149 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>tgt.[dt1]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dif.(src.[dt1] | tgt.[dt1])</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>src.[dt2]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[dt2]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dif.(src.[dt2] | tgt.[dt2])</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>2eb86e3a-3239-440b-8e9f-7ab13604494d</t>
+          <t>171eadc6-bd02-4648-ae29-610644a96833</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>45346d72-b355-48c8-94ed-a907a91c4375</t>
+          <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>12.85265</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>3.109741954</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3.109741954</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>5434643f-0598-4c31-833d-d759fdc14e84</t>
+          <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>b15f70be-cd58-47e1-9fe6-44d7dbadb279</t>
+          <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>8.288637606</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10.49718063</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>5b13b738-5b73-467c-84a7-bc2f8d8d2a47</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>90435b5a-2da5-42d1-9a55-17de4f2bee5a</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>7.575726</v>
+      </c>
+      <c r="G4" t="n">
         <v>7.906586852</v>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>204ee986-cbd8-4666-9dd5-e72ecf7e2535</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>b5733fc5-4403-470f-bcdf-d19eaf7e3dd5</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>8.264160005999999</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.264160005999999</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -956,6 +1062,119 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>src.[pk0] | tgt.[pk0]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>src.[pk1] | tgt.[pk1]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>src.[dt1]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[dt1]</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dif.(src.[dt1] | tgt.[dt1])</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>src.[dt2]</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[dt2]</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dif.(src.[dt2] | tgt.[dt2])</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>027fb2a6-3699-44f5-9030-301eeb682e70</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>bc66fd91-a6ed-4393-abef-b55afe772ad4</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>7.412738474</v>
+      </c>
+      <c r="G2" t="n">
+        <v>7.412738474</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>4c348ab9-4380-4949-80fc-557a1f9bee49</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>a48cfeab-b21a-4e3c-99d9-930cd9075afe</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>8.182236858</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.182236858</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -972,59 +1191,59 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
+          <t>src.[pk0]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
+          <t>src.[pk1]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt1]</t>
+          <t>src.[dt1]</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt2]</t>
+          <t>src.[dt2]</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>3133793a-1301-45de-a590-0e4c74656bca</t>
+          <t>2eb86e3a-3239-440b-8e9f-7ab13604494d</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>90d9c0d6-1a87-47a5-8001-11a8f7c08872</t>
+          <t>45346d72-b355-48c8-94ed-a907a91c4375</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>8.288637606</v>
+        <v>12.85265</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>64442c0b-3005-4e11-bd6b-7c8643ccccdb</t>
+          <t>5434643f-0598-4c31-833d-d759fdc14e84</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>4a584227-220e-4cd9-8fa8-1cb54339a92e</t>
+          <t>b15f70be-cd58-47e1-9fe6-44d7dbadb279</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>10.45706548</v>
+        <v>7.906586852</v>
       </c>
     </row>
   </sheetData>
@@ -1032,7 +1251,84 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[pk0]</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[pk1]</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[dt1]</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tgt.[dt2]</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>3133793a-1301-45de-a590-0e4c74656bca</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>90d9c0d6-1a87-47a5-8001-11a8f7c08872</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8.288637606</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>64442c0b-3005-4e11-bd6b-7c8643ccccdb</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>4a584227-220e-4cd9-8fa8-1cb54339a92e</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10.45706548</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1049,12 +1345,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
+          <t>src.[pk0]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
+          <t>src.[pk1]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1073,7 +1369,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1090,22 +1386,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
+          <t>tgt.[pk0]</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
+          <t>tgt.[pk1]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt1]</t>
+          <t>tgt.[dt1]</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt2]</t>
+          <t>tgt.[dt2]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
* Updated and patched unit tests. * Tests still not working:   - test_field_transform_custom_python   - test_primary_keys_automatch_data_fields   - test_python_edit
</commit_message>
<xml_diff>
--- a/tests/test_artifacts/test_report_excel/benchmarks/test_report_excel.xlsx
+++ b/tests/test_artifacts/test_report_excel/benchmarks/test_report_excel.xlsx
@@ -44,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -57,6 +57,34 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -432,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,110 +471,72 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[column_name] | tgt.[column_name]</t>
+          <t>field_pair</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[native_type]</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[native_type]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[native_type] | tgt.[native_type])</t>
-        </is>
-      </c>
+          <t>native_type | native_type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>src.[py_type]</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[py_type]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[py_type] | tgt.[py_type])</t>
-        </is>
-      </c>
+          <t>py_type | py_type</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>pk0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>OPENPYXL_TYPE_STRING</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>object_</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>object_</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
+          <t>value_type</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>pk1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>OPENPYXL_TYPE_STRING</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>object_</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>object_</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+          <t>column_name | column_name</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>dt0</t>
+          <t>pk0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -579,7 +569,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>dt1</t>
+          <t>pk1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -589,7 +579,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>OPENPYXL_TYPE_NUMERIC</t>
+          <t>OPENPYXL_TYPE_STRING</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -599,12 +589,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>object_</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>object_</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
@@ -612,42 +602,377 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
+          <t>dt0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OPENPYXL_TYPE_STRING</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>object_</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>object_</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>dt1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OPENPYXL_TYPE_NUMERIC</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
           <t>dt2</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>str</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>OPENPYXL_TYPE_NUMERIC</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>float64</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>float64</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>field_pair</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>dt1 | dt1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>dt2 | dt2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>value_type</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>pk0 | pk0</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>pk1 | pk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>027fb2a6-3699-44f5-9030-301eeb682e70</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>bc66fd91-a6ed-4393-abef-b55afe772ad4</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>7.412738474</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.412738474</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>171eadc6-bd02-4648-ae29-610644a96833</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>3.109741954</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.109741954</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>8.288637606</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10.49718063</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>5b13b738-5b73-467c-84a7-bc2f8d8d2a47</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>90435b5a-2da5-42d1-9a55-17de4f2bee5a</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>7.575726</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7.906586852</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>204ee986-cbd8-4666-9dd5-e72ecf7e2535</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>b5733fc5-4403-470f-bcdf-d19eaf7e3dd5</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>8.264160005999999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.264160005999999</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>4c348ab9-4380-4949-80fc-557a1f9bee49</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>a48cfeab-b21a-4e3c-99d9-930cd9075afe</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>8.182236858</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.182236858</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -662,156 +987,128 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
+          <t>field_pair</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt1]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt1]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt1] | tgt.[dt1])</t>
-        </is>
-      </c>
+          <t>dt1 | dt1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt2]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt2]</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt2] | tgt.[dt2])</t>
-        </is>
-      </c>
+          <t>dt2 | dt2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>027fb2a6-3699-44f5-9030-301eeb682e70</t>
-        </is>
-      </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>bc66fd91-a6ed-4393-abef-b55afe772ad4</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>7.412738474</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.412738474</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>value_type</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>171eadc6-bd02-4648-ae29-610644a96833</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>3.109741954</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3.109741954</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>pk1 | pk1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
+          <t>171eadc6-bd02-4648-ae29-610644a96833</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
+          <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>8.288637606</v>
+        <v>3.109741954</v>
       </c>
       <c r="G4" t="n">
-        <v>10.49718063</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
+        <v>3.109741954</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>5b13b738-5b73-467c-84a7-bc2f8d8d2a47</t>
+          <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>90435b5a-2da5-42d1-9a55-17de4f2bee5a</t>
+          <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>7.575726</v>
+        <v>8.288637606</v>
       </c>
       <c r="G5" t="n">
-        <v>7.906586852</v>
+        <v>10.49718063</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -822,65 +1119,73 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>204ee986-cbd8-4666-9dd5-e72ecf7e2535</t>
+          <t>5b13b738-5b73-467c-84a7-bc2f8d8d2a47</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>b5733fc5-4403-470f-bcdf-d19eaf7e3dd5</t>
+          <t>90435b5a-2da5-42d1-9a55-17de4f2bee5a</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>7.575726</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.906586852</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>*</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>8.264160005999999</v>
-      </c>
-      <c r="G6" t="n">
-        <v>8.264160005999999</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>4c348ab9-4380-4949-80fc-557a1f9bee49</t>
+          <t>204ee986-cbd8-4666-9dd5-e72ecf7e2535</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>a48cfeab-b21a-4e3c-99d9-930cd9075afe</t>
+          <t>b5733fc5-4403-470f-bcdf-d19eaf7e3dd5</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
       <c r="F7" t="n">
-        <v>8.182236858</v>
+        <v>8.264160005999999</v>
       </c>
       <c r="G7" t="n">
-        <v>8.182236858</v>
+        <v>8.264160005999999</v>
       </c>
       <c r="H7" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -895,281 +1200,132 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
+          <t>field_pair</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt1]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt1]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt1] | tgt.[dt1])</t>
-        </is>
-      </c>
+          <t>dt1 | dt1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt2]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt2]</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt2] | tgt.[dt2])</t>
-        </is>
-      </c>
+          <t>dt2 | dt2</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>171eadc6-bd02-4648-ae29-610644a96833</t>
-        </is>
-      </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>dd2b12dd-24bd-4bf8-aaa6-d6226b8b8f75</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>3.109741954</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3.109741954</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>value_type</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>target</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>diff</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>0525d9b8-5029-4aeb-9635-4923564a4507</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>15fe2b7d-c967-4989-a098-1b238b406b4e</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>9</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>8.288637606</v>
-      </c>
-      <c r="G3" t="n">
-        <v>10.49718063</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>*</t>
+          <t>pk1 | pk1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>5b13b738-5b73-467c-84a7-bc2f8d8d2a47</t>
+          <t>027fb2a6-3699-44f5-9030-301eeb682e70</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>90435b5a-2da5-42d1-9a55-17de4f2bee5a</t>
+          <t>bc66fd91-a6ed-4393-abef-b55afe772ad4</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>7.575726</v>
+        <v>7.412738474</v>
       </c>
       <c r="G4" t="n">
-        <v>7.906586852</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
+        <v>7.412738474</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>204ee986-cbd8-4666-9dd5-e72ecf7e2535</t>
+          <t>4c348ab9-4380-4949-80fc-557a1f9bee49</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>b5733fc5-4403-470f-bcdf-d19eaf7e3dd5</t>
+          <t>a48cfeab-b21a-4e3c-99d9-930cd9075afe</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>8.264160005999999</v>
+        <v>8.182236858</v>
       </c>
       <c r="G5" t="n">
-        <v>8.264160005999999</v>
+        <v>8.182236858</v>
       </c>
       <c r="H5" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>src.[pk0] | tgt.[pk0]</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>src.[pk1] | tgt.[pk1]</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>src.[dt1]</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt1]</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt1] | tgt.[dt1])</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>src.[dt2]</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>tgt.[dt2]</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>dif.(src.[dt2] | tgt.[dt2])</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>027fb2a6-3699-44f5-9030-301eeb682e70</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>bc66fd91-a6ed-4393-abef-b55afe772ad4</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>7.412738474</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.412738474</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>4c348ab9-4380-4949-80fc-557a1f9bee49</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>a48cfeab-b21a-4e3c-99d9-930cd9075afe</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>8.182236858</v>
-      </c>
-      <c r="G3" t="n">
-        <v>8.182236858</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-    </row>
-  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1191,22 +1347,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk0]</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1]</t>
+          <t>pk1 | pk1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt1]</t>
+          <t>dt1 | dt1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt2]</t>
+          <t>dt2 | dt2</t>
         </is>
       </c>
     </row>
@@ -1268,22 +1424,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[pk0]</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[pk1]</t>
+          <t>pk1 | pk1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt1]</t>
+          <t>dt1 | dt1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt2]</t>
+          <t>dt2 | dt2</t>
         </is>
       </c>
     </row>
@@ -1345,22 +1501,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk0]</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>src.[pk1]</t>
+          <t>pk1 | pk1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt1]</t>
+          <t>dt1 | dt1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>src.[dt2]</t>
+          <t>dt2 | dt2</t>
         </is>
       </c>
     </row>
@@ -1386,22 +1542,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[pk0]</t>
+          <t>pk0 | pk0</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[pk1]</t>
+          <t>pk1 | pk1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt1]</t>
+          <t>dt1 | dt1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>tgt.[dt2]</t>
+          <t>dt2 | dt2</t>
         </is>
       </c>
     </row>

</xml_diff>